<commit_message>
update feb 7 2024
</commit_message>
<xml_diff>
--- a/lecture08_pandas_io/mydata_excel.xlsx
+++ b/lecture08_pandas_io/mydata_excel.xlsx
@@ -1,51 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="s1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="s1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -60,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -376,77 +420,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="n">
+        <v>0.8584253006459687</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.2883171445852273</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="B3" t="n">
+        <v>0.9440780667701379</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5564356437668533</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.3865832100188182</v>
-      </c>
-      <c r="C2">
-        <v>0.4773482093807488</v>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.2196686436106886</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.04393218513957309</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0.6635665375638224</v>
-      </c>
-      <c r="C3">
-        <v>0.3511447300354085</v>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0806535225480115</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.6612488798201234</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0.934059350902934</v>
-      </c>
-      <c r="C4">
-        <v>0.994611217177036</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0.2527665733146013</v>
-      </c>
-      <c r="C5">
-        <v>0.77346621753131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0.1545364252138884</v>
-      </c>
-      <c r="C6">
-        <v>0.8846048007310315</v>
+      <c r="B6" t="n">
+        <v>0.903534649916815</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.9009844779010717</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>